<commit_message>
changing paths for new repo structure
</commit_message>
<xml_diff>
--- a/mappings/outputs-solarchem-mapping.xlsx
+++ b/mappings/outputs-solarchem-mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-kg/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF4360A-3AE9-3B46-A3B3-E33786A36F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8183B2-6F1F-1248-84A7-4FCA1C2F5FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -837,7 +837,7 @@
     <t>{ch3oh_selectivity_molg}</t>
   </si>
   <si>
-    <t>../mappings/data/catalystsdata.csv</t>
+    <t>../data/processed/catalystsdata.csv</t>
   </si>
 </sst>
 </file>
@@ -1427,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3343,7 +3343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H283"/>
   <sheetViews>
-    <sheetView topLeftCell="A261" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C284" sqref="C284"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
queries and figures updated, mappings fixed with minor issues
</commit_message>
<xml_diff>
--- a/mappings/outputs-solarchem-mapping.xlsx
+++ b/mappings/outputs-solarchem-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-kg/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA4DE40-F300-534F-B3BD-7CF2B168A090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073A6FB4-2F24-0847-8574-70B5F693D0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1040" windowWidth="27320" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="1040" windowWidth="27320" windowHeight="21100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -1925,7 +1925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:B18"/>
     </sheetView>
   </sheetViews>
@@ -6011,8 +6011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H465"/>
   <sheetViews>
-    <sheetView topLeftCell="A434" zoomScale="118" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C468" sqref="C468"/>
+    <sheetView tabSelected="1" topLeftCell="A424" zoomScale="118" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C435" sqref="C435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11932,7 +11932,7 @@
       <c r="B437" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C437" t="s">
+      <c r="C437" s="8" t="s">
         <v>154</v>
       </c>
       <c r="D437" t="s">
@@ -12038,7 +12038,7 @@
       <c r="B445" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C445" t="s">
+      <c r="C445" s="8" t="s">
         <v>155</v>
       </c>
       <c r="D445" t="s">
@@ -12144,7 +12144,7 @@
       <c r="B453" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C453" t="s">
+      <c r="C453" s="8" t="s">
         <v>156</v>
       </c>
       <c r="D453" t="s">
@@ -12250,7 +12250,7 @@
       <c r="B461" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C461" t="s">
+      <c r="C461" s="8" t="s">
         <v>165</v>
       </c>
       <c r="D461" t="s">
@@ -12312,6 +12312,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C437" r:id="rId1" xr:uid="{417583C1-8A1D-8C48-A1B6-CA56C82D2F9B}"/>
+    <hyperlink ref="C445" r:id="rId2" xr:uid="{335DF4F1-6AFF-8D45-9015-11D7752A64B5}"/>
+    <hyperlink ref="C453" r:id="rId3" xr:uid="{7F4E54EB-52FF-0E4A-AE12-4D5484BC8082}"/>
+    <hyperlink ref="C461" r:id="rId4" xr:uid="{153C3496-D712-704D-8289-A6D98937227A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>